<commit_message>
Fetching wi-fi networks working
</commit_message>
<xml_diff>
--- a/Source/ews/Documents/External/Common/EWS000003 Traceability Matrix Easy WiFi Setup UX.xlsx
+++ b/Source/ews/Documents/External/Common/EWS000003 Traceability Matrix Easy WiFi Setup UX.xlsx
@@ -888,34 +888,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1C11274C-892B-5F42-AF43-BB68D21B4EEF}" diskRevisions="1" revisionId="18" version="2">
-  <header guid="{1A553375-48A2-9244-A11E-9A3320265BCF}" dateTime="2017-11-17T15:09:12" maxSheetId="4" userName="Microsoft Office User" r:id="rId1">
-    <sheetIdMap count="3">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{03823957-A7D6-514D-BF89-4CD73B0C21CD}" dateTime="2017-11-17T15:11:18" maxSheetId="4" userName="Microsoft Office User" r:id="rId2" minRId="1">
-    <sheetIdMap count="3">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{A41C3A18-8DEE-BC4C-B029-0D0E49D0418F}" dateTime="2017-11-20T13:14:05" maxSheetId="4" userName="Microsoft Office User" r:id="rId3" minRId="2">
-    <sheetIdMap count="3">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{4C95D876-1258-F548-9502-2CF738DD597D}" dateTime="2017-11-20T13:25:01" maxSheetId="4" userName="Microsoft Office User" r:id="rId4" minRId="3" maxRId="7">
-    <sheetIdMap count="3">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-    </sheetIdMap>
-  </header>
   <header guid="{1C11274C-892B-5F42-AF43-BB68D21B4EEF}" dateTime="2017-12-07T15:31:47" maxSheetId="4" userName="Microsoft Office User" r:id="rId5" minRId="8" maxRId="18">
     <sheetIdMap count="3">
       <sheetId val="1"/>
@@ -924,183 +896,6 @@
     </sheetIdMap>
   </header>
 </headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rrc rId="1" sId="2" ref="A109:XFD109" action="deleteRow">
-    <rfmt sheetId="2" xfDxf="1" sqref="A109:XFD109" start="0" length="0">
-      <dxf>
-        <font>
-          <name val="Arial"/>
-          <scheme val="none"/>
-        </font>
-        <alignment horizontal="left" vertical="top" readingOrder="0"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="2" dxf="1">
-      <nc r="A109" t="inlineStr">
-        <is>
-          <t>37455</t>
-        </is>
-      </nc>
-      <ndxf>
-        <font>
-          <sz val="11"/>
-          <color theme="1"/>
-          <name val="Calibri"/>
-          <scheme val="minor"/>
-        </font>
-        <alignment wrapText="1" readingOrder="0"/>
-      </ndxf>
-    </rcc>
-    <rcc rId="0" sId="2" dxf="1">
-      <nc r="B109" t="inlineStr">
-        <is>
-          <t>Technical Interfaces</t>
-        </is>
-      </nc>
-      <ndxf>
-        <font>
-          <sz val="11"/>
-          <color theme="1"/>
-          <name val="Calibri"/>
-          <scheme val="minor"/>
-        </font>
-        <alignment wrapText="1" readingOrder="0"/>
-      </ndxf>
-    </rcc>
-    <rfmt sheetId="2" sqref="C109" start="0" length="0">
-      <dxf>
-        <font>
-          <sz val="11"/>
-          <color theme="1"/>
-          <name val="Calibri"/>
-          <scheme val="minor"/>
-        </font>
-        <alignment wrapText="1" readingOrder="0"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="2" sqref="D109" start="0" length="0">
-      <dxf>
-        <font>
-          <sz val="11"/>
-          <color theme="1"/>
-          <name val="Calibri"/>
-          <scheme val="minor"/>
-        </font>
-        <alignment wrapText="1" readingOrder="0"/>
-      </dxf>
-    </rfmt>
-  </rrc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="2" sId="1">
-    <oc r="A6" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>This Requirement Traceability Matrix is applicable for the work done in release PI 17.5.</t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="11"/>
-            <color theme="5"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-      </is>
-    </oc>
-    <nc r="A6" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>This Requirement Traceability Matrix is applicable for the work done in Platform Release 2017.5.0.</t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="11"/>
-            <color theme="5"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{B643A179-4F56-C84F-B243-C8CAAA56860F}" action="delete"/>
-  <rcv guid="{B643A179-4F56-C84F-B243-C8CAAA56860F}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="3" sId="3">
-    <nc r="A5" t="inlineStr">
-      <is>
-        <t>0.1</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="3" sqref="B5" start="0" length="0">
-    <dxf>
-      <font>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="4" sId="3" numFmtId="19">
-    <nc r="B5">
-      <v>43059</v>
-    </nc>
-  </rcc>
-  <rcc rId="5" sId="3">
-    <nc r="C5" t="inlineStr">
-      <is>
-        <t>Lynn Slooten</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="6" sId="3">
-    <nc r="D5" t="inlineStr">
-      <is>
-        <t>Changed release name</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="7" sId="3">
-    <nc r="E5" t="inlineStr">
-      <is>
-        <t>release name was incorrect</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Revert back from develop
</commit_message>
<xml_diff>
--- a/Source/ews/Documents/External/Common/EWS000003 Traceability Matrix Easy WiFi Setup UX.xlsx
+++ b/Source/ews/Documents/External/Common/EWS000003 Traceability Matrix Easy WiFi Setup UX.xlsx
@@ -888,6 +888,34 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1C11274C-892B-5F42-AF43-BB68D21B4EEF}" diskRevisions="1" revisionId="18" version="2">
+  <header guid="{1A553375-48A2-9244-A11E-9A3320265BCF}" dateTime="2017-11-17T15:09:12" maxSheetId="4" userName="Microsoft Office User" r:id="rId1">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{03823957-A7D6-514D-BF89-4CD73B0C21CD}" dateTime="2017-11-17T15:11:18" maxSheetId="4" userName="Microsoft Office User" r:id="rId2" minRId="1">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A41C3A18-8DEE-BC4C-B029-0D0E49D0418F}" dateTime="2017-11-20T13:14:05" maxSheetId="4" userName="Microsoft Office User" r:id="rId3" minRId="2">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{4C95D876-1258-F548-9502-2CF738DD597D}" dateTime="2017-11-20T13:25:01" maxSheetId="4" userName="Microsoft Office User" r:id="rId4" minRId="3" maxRId="7">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
   <header guid="{1C11274C-892B-5F42-AF43-BB68D21B4EEF}" dateTime="2017-12-07T15:31:47" maxSheetId="4" userName="Microsoft Office User" r:id="rId5" minRId="8" maxRId="18">
     <sheetIdMap count="3">
       <sheetId val="1"/>
@@ -896,6 +924,183 @@
     </sheetIdMap>
   </header>
 </headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="1" sId="2" ref="A109:XFD109" action="deleteRow">
+    <rfmt sheetId="2" xfDxf="1" sqref="A109:XFD109" start="0" length="0">
+      <dxf>
+        <font>
+          <name val="Arial"/>
+          <scheme val="none"/>
+        </font>
+        <alignment horizontal="left" vertical="top" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2" dxf="1">
+      <nc r="A109" t="inlineStr">
+        <is>
+          <t>37455</t>
+        </is>
+      </nc>
+      <ndxf>
+        <font>
+          <sz val="11"/>
+          <color theme="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment wrapText="1" readingOrder="0"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="2" dxf="1">
+      <nc r="B109" t="inlineStr">
+        <is>
+          <t>Technical Interfaces</t>
+        </is>
+      </nc>
+      <ndxf>
+        <font>
+          <sz val="11"/>
+          <color theme="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment wrapText="1" readingOrder="0"/>
+      </ndxf>
+    </rcc>
+    <rfmt sheetId="2" sqref="C109" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color theme="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment wrapText="1" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" sqref="D109" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="11"/>
+          <color theme="1"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+        <alignment wrapText="1" readingOrder="0"/>
+      </dxf>
+    </rfmt>
+  </rrc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="2" sId="1">
+    <oc r="A6" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>This Requirement Traceability Matrix is applicable for the work done in release PI 17.5.</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="11"/>
+            <color theme="5"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+      </is>
+    </oc>
+    <nc r="A6" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>This Requirement Traceability Matrix is applicable for the work done in Platform Release 2017.5.0.</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="11"/>
+            <color theme="5"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{B643A179-4F56-C84F-B243-C8CAAA56860F}" action="delete"/>
+  <rcv guid="{B643A179-4F56-C84F-B243-C8CAAA56860F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="3" sId="3">
+    <nc r="A5" t="inlineStr">
+      <is>
+        <t>0.1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="3" sqref="B5" start="0" length="0">
+    <dxf>
+      <font>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="4" sId="3" numFmtId="19">
+    <nc r="B5">
+      <v>43059</v>
+    </nc>
+  </rcc>
+  <rcc rId="5" sId="3">
+    <nc r="C5" t="inlineStr">
+      <is>
+        <t>Lynn Slooten</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="6" sId="3">
+    <nc r="D5" t="inlineStr">
+      <is>
+        <t>Changed release name</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="7" sId="3">
+    <nc r="E5" t="inlineStr">
+      <is>
+        <t>release name was incorrect</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>